<commit_message>
fix: Regenerate Excel template and redesign HTML guide with document styling
</commit_message>
<xml_diff>
--- a/backend/static/templates/Retirement_Analysis_Template.xlsx
+++ b/backend/static/templates/Retirement_Analysis_Template.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="Raw Data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Summary Dashboard" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Top Scenarios" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Scenario Comparison" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Instructions" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,12 +18,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="70AD47"/>
-    <numFmt numFmtId="165" formatCode="FF0000"/>
-    <numFmt numFmtId="166" formatCode="$#,##0"/>
-  </numFmts>
-  <fonts count="10">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -38,39 +33,24 @@
       <sz val="11"/>
     </font>
     <font>
-      <b val="1"/>
-      <color rgb="00FF0000"/>
-      <sz val="12"/>
+      <i val="1"/>
+      <color rgb="00666666"/>
     </font>
     <font>
       <b val="1"/>
-      <color rgb="002F5496"/>
-      <sz val="18"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="14"/>
+      <color rgb="002E5C8A"/>
+      <sz val="16"/>
     </font>
     <font>
       <b val="1"/>
     </font>
     <font>
-      <i val="1"/>
-    </font>
-    <font>
       <b val="1"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
-    <font>
-      <i val="1"/>
-      <sz val="10"/>
+      <color rgb="002E5C8A"/>
+      <sz val="12"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -81,24 +61,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0070AD47"/>
-        <bgColor rgb="0070AD47"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFF2CC"/>
-        <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -114,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -123,20 +85,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -502,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,7 +458,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="20" customHeight="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>scenario_id</t>
@@ -638,84 +586,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>65</v>
-      </c>
-      <c r="C2" t="n">
-        <v>100000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>30000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>60000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>65</v>
-      </c>
-      <c r="N2" t="n">
-        <v>65</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>55</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>100000</v>
-      </c>
-      <c r="R2" t="n">
-        <v>30000</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>130000</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="b">
-        <v>1</v>
-      </c>
-      <c r="X2" t="n">
-        <v>50000</v>
-      </c>
-      <c r="Y2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>👉 PASTE YOUR CSV DATA HERE (starting at row 2, replacing the sample)</t>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>👇 Paste your CSV data starting from row 3</t>
         </is>
       </c>
     </row>
@@ -730,175 +603,29 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>🎯 Retirement Scenario Analysis</t>
+          <t>📊 Retirement Analysis Summary</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>📊 Key Metrics</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t>Total Scenarios:</t>
-        </is>
-      </c>
-      <c r="B5">
-        <f>COUNTA('Raw Data'!A:A)-2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>Unique Scenarios:</t>
-        </is>
-      </c>
-      <c r="B6">
-        <f>MAX('Raw Data'!A:A)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Successful Plans:</t>
-        </is>
-      </c>
-      <c r="B7" s="6">
-        <f>COUNTIF('Raw Data'!W:W,TRUE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Failed Plans:</t>
-        </is>
-      </c>
-      <c r="B8" s="7">
-        <f>COUNTIF('Raw Data'!W:W,FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>Success Rate:</t>
-        </is>
-      </c>
-      <c r="B9" s="8">
-        <f>B6/(B6+B7)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>Avg Final Balance:</t>
-        </is>
-      </c>
-      <c r="B10" s="9">
-        <f>AVERAGEIF('Raw Data'!W:W,TRUE,'Raw Data'!X:X)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>📖 Quick Start Guide</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1. Paste CSV data into 'Raw Data' sheet (starting row 2)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2. This dashboard auto-updates with your results</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>3. Go to 'Top Scenarios' to see best outcomes</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>4. Use 'Scenario Comparison' for detailed analysis</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>5. Filter 'Raw Data' by success=TRUE to see viable plans</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>💡 Tips:</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • Sort by final_balance (column X) to find best scenarios</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • Filter by retirement_age to compare retirement timing</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • Check warnings column for issues in failed scenarios</t>
+          <t>Best Scenarios (Success Rate):</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -909,130 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="11" t="inlineStr">
-        <is>
-          <t>🏆 Top 10 Successful Scenarios</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t>Rank</t>
-        </is>
-      </c>
-      <c r="B3" s="12" t="inlineStr">
-        <is>
-          <t>Scenario ID</t>
-        </is>
-      </c>
-      <c r="C3" s="12" t="inlineStr">
-        <is>
-          <t>Final Balance</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="inlineStr">
-        <is>
-          <t>Retirement Age</t>
-        </is>
-      </c>
-      <c r="E3" s="12" t="inlineStr">
-        <is>
-          <t>RRSP Start</t>
-        </is>
-      </c>
-      <c r="F3" s="12" t="inlineStr">
-        <is>
-          <t>TFSA Start</t>
-        </is>
-      </c>
-      <c r="G3" s="12" t="inlineStr">
-        <is>
-          <t>Annual Spending</t>
-        </is>
-      </c>
-      <c r="H3" s="12" t="inlineStr">
-        <is>
-          <t>Pensions</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>📋 Instructions:</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1. Go to Raw Data sheet</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2. Select all data (Ctrl+A)</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>3. Data → Sort → Sort by 'final_balance' descending</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>4. Filter 'success' column to TRUE only</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>5. Copy top 10 rows here manually (or use pivot table)</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1041,106 +645,161 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="inlineStr">
-        <is>
-          <t>📊 Compare Up To 5 Scenarios</t>
-        </is>
-      </c>
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>📋 How to Use This Template</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>Enter Scenario IDs to compare:</t>
+          <t>Step 1: Download your CSV</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="13" t="inlineStr">
-        <is>
-          <t>Scenario 1</t>
-        </is>
-      </c>
-      <c r="C4" s="13" t="inlineStr">
-        <is>
-          <t>Scenario 2</t>
-        </is>
-      </c>
-      <c r="D4" s="13" t="inlineStr">
-        <is>
-          <t>Scenario 3</t>
-        </is>
-      </c>
-      <c r="E4" s="13" t="inlineStr">
-        <is>
-          <t>Scenario 4</t>
-        </is>
-      </c>
-      <c r="F4" s="13" t="inlineStr">
-        <is>
-          <t>Scenario 5</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Run batch analysis on https://retirement-planning-dapp.vercel.app</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="14" t="n"/>
-      <c r="C5" s="14" t="n"/>
-      <c r="D5" s="14" t="n"/>
-      <c r="E5" s="14" t="n"/>
-      <c r="F5" s="14" t="n"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Complete Solana payment</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Download the CSV file</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Retirement Age</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>Starting RRSP</t>
+          <t>Step 2: Import CSV data</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>Starting TFSA</t>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Open the CSV file in Excel or text editor</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>Annual Spending</t>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Copy ALL rows (including header)</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="inlineStr">
-        <is>
-          <t>Final Balance</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Go to 'Raw Data' sheet</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>Success?</t>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Paste starting at cell A1 (overwrite existing header)</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="inlineStr">
-        <is>
-          <t>Years to Depletion</t>
+      <c r="A13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>Step 3: Analyze results</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="15" t="inlineStr">
-        <is>
-          <t>Use VLOOKUP or XLOOKUP to pull data from Raw Data sheet</t>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Summary Dashboard: See key metrics</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Use filters to find optimal scenarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Sort by 'success' column (TRUE = plan works)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Compare 'final_balance' to see how much remains</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Key Columns:</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • success: Does retirement plan work? (TRUE/FALSE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • final_balance: Money left at end of life</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • warnings: Why plan failed (if applicable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • num_pensions: Number of pensions in scenario</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • num_properties: Number of properties in scenario</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Add auto-scroll to downloads, populate Excel dashboard with formulas
</commit_message>
<xml_diff>
--- a/backend/static/templates/Retirement_Analysis_Template.xlsx
+++ b/backend/static/templates/Retirement_Analysis_Template.xlsx
@@ -18,8 +18,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="6">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+  </numFmts>
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,8 +52,43 @@
       <color rgb="002E5C8A"/>
       <sz val="12"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="002E5C8A"/>
+      <sz val="18"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <color rgb="00666666"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="0027ae60"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="003498db"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00f39c12"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="008e44ad"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <color rgb="00999999"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -61,6 +99,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00e8f8f5"/>
+        <bgColor rgb="00e8f8f5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ebf5fb"/>
+        <bgColor rgb="00ebf5fb"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00fef5e7"/>
+        <bgColor rgb="00fef5e7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00f4ecf7"/>
+        <bgColor rgb="00f4ecf7"/>
       </patternFill>
     </fill>
   </fills>
@@ -76,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -85,6 +147,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -603,29 +675,205 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>📊 Retirement Analysis Summary</t>
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>📊 Retirement Analysis Dashboard</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>Best Scenarios (Success Rate):</t>
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>After pasting CSV data into 'Raw Data' sheet, this dashboard will auto-update.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>Success Rate Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Total Scenarios:</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA('Raw Data'!A:A)-1</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Successful Scenarios:</t>
+        </is>
+      </c>
+      <c r="B7">
+        <f>COUNTIF('Raw Data'!W:W,TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Success Rate:</t>
+        </is>
+      </c>
+      <c r="B8" s="9">
+        <f>IF(B6&gt;0,B7/B6,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>Financial Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Average Final Balance (Success):</t>
+        </is>
+      </c>
+      <c r="B11" s="11">
+        <f>AVERAGEIF('Raw Data'!W:W,TRUE,'Raw Data'!X:X)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Median Retirement Age (Success):</t>
+        </is>
+      </c>
+      <c r="B12" s="12">
+        <f>MEDIAN(IF('Raw Data'!W:W=TRUE,'Raw Data'!B:B))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Average Annual Spending:</t>
+        </is>
+      </c>
+      <c r="B13" s="11">
+        <f>AVERAGE('Raw Data'!F:F)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="13" t="inlineStr">
+        <is>
+          <t>🏆 Best Scenario</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Best Scenario ID:</t>
+        </is>
+      </c>
+      <c r="B16">
+        <f>INDEX('Raw Data'!A:A,MATCH(MAX(IF('Raw Data'!W:W=TRUE,'Raw Data'!X:X)),IF('Raw Data'!W:W=TRUE,'Raw Data'!X:X),0)+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Final Balance:</t>
+        </is>
+      </c>
+      <c r="B17" s="11">
+        <f>MAX(IF('Raw Data'!W:W=TRUE,'Raw Data'!X:X))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Retirement Age:</t>
+        </is>
+      </c>
+      <c r="B18">
+        <f>INDEX('Raw Data'!B:B,MATCH(MAX(IF('Raw Data'!W:W=TRUE,'Raw Data'!X:X)),IF('Raw Data'!W:W=TRUE,'Raw Data'!X:X),0)+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="14" t="inlineStr">
+        <is>
+          <t>�� Key Insights</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Scenarios with Pensions:</t>
+        </is>
+      </c>
+      <c r="B21">
+        <f>COUNTIF('Raw Data'!L:L,"&gt;0")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Scenarios with Properties:</t>
+        </is>
+      </c>
+      <c r="B22">
+        <f>COUNTIF('Raw Data'!K:K,"&gt;0")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Average Tax Paid (per year):</t>
+        </is>
+      </c>
+      <c r="B23" s="11">
+        <f>AVERAGE('Raw Data'!V:V)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="15" t="inlineStr">
+        <is>
+          <t>Note: Some formulas use array logic. Press Ctrl+Shift+Enter when editing them.</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -651,9 +899,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
@@ -682,9 +928,7 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-    </row>
+    <row r="7"/>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
@@ -720,9 +964,7 @@
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-    </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
@@ -758,9 +1000,7 @@
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-    </row>
+    <row r="19"/>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fix: Zero num_pensions when unchecked, add Excel chart guides, fix paste instructions
</commit_message>
<xml_diff>
--- a/backend/static/templates/Retirement_Analysis_Template.xlsx
+++ b/backend/static/templates/Retirement_Analysis_Template.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Raw Data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Summary Dashboard" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Instructions" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Chart Templates" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -22,7 +23,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="22">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -87,8 +88,50 @@
       <color rgb="00999999"/>
       <sz val="9"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <color rgb="00E74C3C"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="0016a085"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="002980b9"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="0027ae60"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00e67e22"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="009b59b6"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -125,6 +168,12 @@
         <bgColor rgb="00f4ecf7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00e8f6f3"/>
+        <bgColor rgb="00e8f6f3"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -138,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -157,6 +206,15 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -658,9 +716,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>👇 Paste your CSV data starting from row 3</t>
+      <c r="A2" s="16" t="inlineStr">
+        <is>
+          <t>👆 PASTE ENTIRE CSV HERE - Select cell A1, then Ctrl+V (overwrites header)</t>
         </is>
       </c>
     </row>
@@ -675,7 +733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -865,6 +923,177 @@
       <c r="A25" s="15" t="inlineStr">
         <is>
           <t>Note: Some formulas use array logic. Press Ctrl+Shift+Enter when editing them.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="17" t="inlineStr">
+        <is>
+          <t>📈 Visual Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="18" t="inlineStr">
+        <is>
+          <t>Chart 1: Best Scenario Balance Over Time</t>
+        </is>
+      </c>
+      <c r="D28" s="15" t="inlineStr">
+        <is>
+          <t>← Charts will appear here after you create them</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="18" t="inlineStr">
+        <is>
+          <t>Chart 2: Compare Two Scenarios (Optional)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="19" t="inlineStr">
+        <is>
+          <t>📋 How to Create Charts:</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="20" t="inlineStr">
+        <is>
+          <t>Chart 1 - Best Scenario:</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1. Go to 'Raw Data' sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  2. Filter column A (scenario_id) to show only the best scenario</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  3. Select columns: 'age' and 'total_balance'</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  4. Insert → Chart → Line Chart</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  5. Title: 'Best Scenario - Balance Over Time'</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="20" t="inlineStr">
+        <is>
+          <t>Chart 2 - Compare Scenarios (Optional):</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1. Filter to show TWO scenario IDs</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  2. Select 'age', 'total_balance' for both</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  3. Insert → Line Chart with 2 data series</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  4. Use different colors for each scenario</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Quick Tip:</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • After pasting CSV, find best scenario ID in cell B16</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Filter Raw Data by that scenario_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Create chart from filtered data</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Power User Tip:</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Pivot table by scenario_id to compare multiple plans</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Use conditional formatting to highlight age when balance drops below threshold</t>
         </is>
       </c>
     </row>
@@ -899,7 +1128,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
@@ -928,7 +1156,6 @@
         </is>
       </c>
     </row>
-    <row r="7"/>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
@@ -964,7 +1191,6 @@
         </is>
       </c>
     </row>
-    <row r="13"/>
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
@@ -1000,46 +1226,281 @@
         </is>
       </c>
     </row>
-    <row r="19"/>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>Step 4: Create Charts (Optional)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • See 'Chart Templates' sheet for detailed instructions</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Quick: Filter by best scenario → Select age + total_balance → Insert Chart</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Charts help visualize balance over time</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • num_properties: Number of properties in scenario</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="70" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>📊 Ready-to-Use Chart Templates</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="22" t="inlineStr">
+        <is>
+          <t>Instructions:</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>After pasting your CSV into 'Raw Data':</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="23" t="inlineStr">
+        <is>
+          <t>Option A - Automatic Chart (Recommended):</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1. Copy best scenario_id from Dashboard (cell B16)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  2. Go to Raw Data sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  3. Click the filter dropdown in column A (scenario_id)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  4. Paste the scenario ID, click OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  5. Select columns P (age) and T (total_balance)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  6. Insert → Chart → Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  7. Move chart to Dashboard sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="23" t="inlineStr">
+        <is>
+          <t>Option B - Compare Two Scenarios:</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1. Filter Raw Data to show 2 scenario IDs</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  2. Select age and total_balance columns</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  3. Insert → Line Chart</t>
+        </is>
+      </c>
+    </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Key Columns:</t>
+          <t xml:space="preserve">  4. Excel will create 2 series automatically</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">   • success: Does retirement plan work? (TRUE/FALSE)</t>
+          <t xml:space="preserve">  5. Format: Different colors, add legend</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • final_balance: Money left at end of life</t>
-        </is>
-      </c>
+      <c r="A22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • warnings: Why plan failed (if applicable)</t>
+      <c r="A23" s="24" t="inlineStr">
+        <is>
+          <t>Column Reference:</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">   • num_pensions: Number of pensions in scenario</t>
+          <t xml:space="preserve">  • Column A = scenario_id</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">   • num_properties: Number of properties in scenario</t>
+          <t xml:space="preserve">  • Column P = age (X-axis)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Column T = total_balance (Y-axis)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Column U = gross_income (optional Y-axis)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Column V = taxes_estimated (optional Y-axis)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="24" t="inlineStr">
+        <is>
+          <t>Chart Formatting Tips:</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Title: 'Retirement Balance Projection'</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • X-axis: Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Y-axis: Balance ($)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Line style: Smooth curves</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Add data labels for key milestones (optional)</t>
         </is>
       </c>
     </row>

</xml_diff>